<commit_message>
Ran Strategy 2 for all elections
</commit_message>
<xml_diff>
--- a/results/Year & Strategy Comparison.xlsx
+++ b/results/Year & Strategy Comparison.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Documents/dev/MM2/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738EF8DE-5FA2-9E48-A507-F8CD3FDDD3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B1B4D6-C128-F745-BD61-AE8510ABA023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="10120" windowWidth="28040" windowHeight="17440" xr2:uid="{FDB991F3-65B7-2442-88EF-AF8858A1CE50}"/>
+    <workbookView xWindow="1120" yWindow="500" windowWidth="27680" windowHeight="17500" xr2:uid="{FDB991F3-65B7-2442-88EF-AF8858A1CE50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t>Year</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>stdev</t>
+  </si>
+  <si>
+    <t>Strategy 2</t>
   </si>
 </sst>
 </file>
@@ -381,12 +384,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -400,7 +401,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -415,15 +416,14 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,569 +738,713 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5BCF68F-9CA1-1A41-B9FD-C7E5B292FD92}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M18" sqref="M18"/>
+      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="7.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="5.83203125" customWidth="1"/>
     <col min="6" max="6" width="5.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.83203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="5.83203125" customWidth="1"/>
+    <col min="7" max="8" width="5.83203125" customWidth="1"/>
     <col min="9" max="9" width="5.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="5.83203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="5.83203125" customWidth="1"/>
-    <col min="12" max="12" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.83203125" customWidth="1"/>
+    <col min="12" max="12" width="5.83203125" style="1" customWidth="1"/>
+    <col min="13" max="14" width="5.83203125" customWidth="1"/>
+    <col min="15" max="15" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="8" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="9" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="9" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="6"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="2"/>
-    </row>
-    <row r="2" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="N1" s="10"/>
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="25">
+    <row r="3" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="23">
         <v>2000</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="24">
         <v>0.503</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="25">
         <v>212</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="25">
         <v>433</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="25">
         <v>6</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="26">
         <v>23</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="25">
         <v>35</v>
       </c>
-      <c r="H3" s="27">
+      <c r="H3" s="25">
         <v>470</v>
       </c>
-      <c r="I3" s="28">
+      <c r="I3" s="26">
+        <v>11</v>
+      </c>
+      <c r="J3" s="25">
+        <v>11</v>
+      </c>
+      <c r="K3" s="25">
+        <v>446</v>
+      </c>
+      <c r="L3" s="26">
         <v>12</v>
       </c>
-      <c r="J3" s="29">
+      <c r="M3" s="25">
         <v>13</v>
       </c>
-      <c r="K3" s="30">
+      <c r="N3" s="27">
         <v>448</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="O3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="13">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="11">
         <v>2002</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>0.48270000000000002</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4">
         <v>205</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4">
         <v>434</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4">
         <v>4</v>
       </c>
       <c r="F4" s="1">
         <v>29</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4">
         <v>51</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4">
         <v>486</v>
       </c>
       <c r="I4" s="1">
+        <v>8</v>
+      </c>
+      <c r="J4" s="34">
+        <v>8</v>
+      </c>
+      <c r="K4" s="34">
+        <v>443</v>
+      </c>
+      <c r="L4" s="1">
         <v>9</v>
       </c>
-      <c r="J4" s="4">
+      <c r="M4">
         <v>10</v>
       </c>
-      <c r="K4" s="14">
+      <c r="N4" s="12">
         <v>445</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="O4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="13">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="11">
         <v>2004</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>0.4919</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <v>201</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5">
         <v>434</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5">
         <v>12</v>
       </c>
       <c r="F5" s="1">
         <v>44</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5">
         <v>65</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5">
         <v>500</v>
       </c>
       <c r="I5" s="1">
+        <v>24</v>
+      </c>
+      <c r="J5" s="34">
+        <v>24</v>
+      </c>
+      <c r="K5" s="34">
+        <v>459</v>
+      </c>
+      <c r="L5" s="1">
         <v>28</v>
       </c>
-      <c r="J5" s="4">
+      <c r="M5">
         <v>32</v>
       </c>
-      <c r="K5" s="14">
+      <c r="N5" s="12">
         <v>467</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="O5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="13">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="11">
         <v>2006</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="3">
         <v>0.54039999999999999</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>233</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6">
         <v>435</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6">
         <v>2</v>
       </c>
       <c r="F6" s="1">
         <v>167</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6">
         <v>306</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6">
         <v>741</v>
       </c>
       <c r="I6" s="1">
+        <v>4</v>
+      </c>
+      <c r="J6" s="34">
+        <v>4</v>
+      </c>
+      <c r="K6" s="34">
+        <v>439</v>
+      </c>
+      <c r="L6" s="1">
         <v>5</v>
       </c>
-      <c r="J6" s="4">
+      <c r="M6">
         <v>6</v>
       </c>
-      <c r="K6" s="14">
+      <c r="N6" s="12">
         <v>441</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="O6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="13">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="11">
         <v>2008</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="3">
         <v>0.55289999999999995</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7">
         <v>257</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7">
         <v>435</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7">
         <v>-16</v>
       </c>
       <c r="F7" s="1">
         <v>57</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7">
         <v>132</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7">
         <v>567</v>
       </c>
       <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="34">
+        <v>29</v>
+      </c>
+      <c r="K7" s="34">
+        <v>464</v>
+      </c>
+      <c r="L7" s="1">
         <v>9</v>
       </c>
-      <c r="J7" s="4">
+      <c r="M7">
         <v>46</v>
       </c>
-      <c r="K7" s="14">
+      <c r="N7" s="12">
         <v>481</v>
       </c>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="31">
+      <c r="O7"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="28">
         <v>2010</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="29">
         <v>0.4723</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="30">
         <v>193</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="30">
         <v>435</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="30">
         <v>12</v>
       </c>
-      <c r="F8" s="34">
+      <c r="F8" s="31">
         <v>54</v>
       </c>
-      <c r="G8" s="35">
+      <c r="G8" s="30">
         <v>89</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="30">
         <v>524</v>
       </c>
-      <c r="I8" s="34">
+      <c r="I8" s="31">
+        <v>23</v>
+      </c>
+      <c r="J8" s="30">
+        <v>23</v>
+      </c>
+      <c r="K8" s="30">
+        <v>458</v>
+      </c>
+      <c r="L8" s="31">
         <v>29</v>
       </c>
-      <c r="J8" s="35">
+      <c r="M8" s="30">
         <v>36</v>
       </c>
-      <c r="K8" s="36">
+      <c r="N8" s="32">
         <v>471</v>
       </c>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="13">
+      <c r="O8"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="11">
         <v>2012</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="3">
         <v>0.50849999999999995</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9">
         <v>201</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9">
         <v>435</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9">
         <v>20</v>
       </c>
       <c r="F9" s="1">
         <v>106</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9">
         <v>169</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9">
         <v>604</v>
       </c>
       <c r="I9" s="1">
+        <v>41</v>
+      </c>
+      <c r="J9" s="34">
+        <v>41</v>
+      </c>
+      <c r="K9" s="34">
+        <v>476</v>
+      </c>
+      <c r="L9" s="1">
         <v>54</v>
       </c>
-      <c r="J9" s="4">
+      <c r="M9">
         <v>67</v>
       </c>
-      <c r="K9" s="14">
+      <c r="N9" s="12">
         <v>502</v>
       </c>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="13">
+      <c r="O9"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="11">
         <v>2014</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="3">
         <v>0.47439999999999999</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10">
         <v>188</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10">
         <v>435</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10">
         <v>18</v>
       </c>
       <c r="F10" s="1">
         <v>88</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10">
         <v>147</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10">
         <v>582</v>
       </c>
       <c r="I10" s="1">
+        <v>34</v>
+      </c>
+      <c r="J10" s="34">
+        <v>34</v>
+      </c>
+      <c r="K10" s="34">
+        <v>469</v>
+      </c>
+      <c r="L10" s="1">
         <v>50</v>
       </c>
-      <c r="J10" s="4">
+      <c r="M10">
         <v>67</v>
       </c>
-      <c r="K10" s="14">
+      <c r="N10" s="12">
         <v>502</v>
       </c>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="13">
+      <c r="O10"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="11">
         <v>2016</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="3">
         <v>0.49530000000000002</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11">
         <v>194</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11">
         <v>435</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11">
         <v>21</v>
       </c>
       <c r="F11" s="1">
         <v>108</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11">
         <v>175</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11">
         <v>610</v>
       </c>
       <c r="I11" s="1">
+        <v>42</v>
+      </c>
+      <c r="J11" s="34">
+        <v>42</v>
+      </c>
+      <c r="K11" s="34">
+        <v>477</v>
+      </c>
+      <c r="L11" s="1">
         <v>53</v>
       </c>
-      <c r="J11" s="4">
+      <c r="M11">
         <v>64</v>
       </c>
-      <c r="K11" s="14">
+      <c r="N11" s="12">
         <v>499</v>
       </c>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="13">
+      <c r="O11"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="11">
         <v>2018</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="3">
         <v>0.5333</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12">
         <v>235</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12">
         <v>434</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12">
         <v>-4</v>
       </c>
       <c r="F12" s="1">
         <v>41</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12">
         <v>83</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12">
         <v>518</v>
       </c>
       <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="34">
+        <v>6</v>
+      </c>
+      <c r="K12" s="34">
+        <v>441</v>
+      </c>
+      <c r="L12" s="1">
         <v>7</v>
       </c>
-      <c r="J12" s="4">
+      <c r="M12">
         <v>19</v>
       </c>
-      <c r="K12" s="14">
+      <c r="N12" s="12">
         <v>454</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="O12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="31">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="28">
         <v>2020</v>
       </c>
-      <c r="B13" s="32">
+      <c r="B13" s="29">
         <v>0.50680000000000003</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13" s="30">
         <v>222</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="30">
         <v>435</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="30">
         <v>-2</v>
       </c>
-      <c r="F13" s="34">
+      <c r="F13" s="31">
         <v>6</v>
       </c>
-      <c r="G13" s="35">
+      <c r="G13" s="30">
         <v>14</v>
       </c>
-      <c r="H13" s="35">
+      <c r="H13" s="30">
         <v>449</v>
       </c>
-      <c r="I13" s="34">
+      <c r="I13" s="31">
+        <v>0</v>
+      </c>
+      <c r="J13" s="30">
+        <v>3</v>
+      </c>
+      <c r="K13" s="30">
+        <v>438</v>
+      </c>
+      <c r="L13" s="31">
         <v>4</v>
       </c>
-      <c r="J13" s="35">
+      <c r="M13" s="30">
         <v>10</v>
       </c>
-      <c r="K13" s="36">
+      <c r="N13" s="32">
         <v>445</v>
       </c>
-      <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
+      <c r="O13"/>
+    </row>
+    <row r="14" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
         <v>2022</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="3"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G16" s="3" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="17"/>
+      <c r="O14"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
         <v>15</v>
       </c>
       <c r="H16">
         <f>MIN(H$3:H$14)</f>
         <v>449</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J16" t="s">
         <v>15</v>
       </c>
       <c r="K16">
         <f>MIN(K$3:K$14)</f>
+        <v>438</v>
+      </c>
+      <c r="M16" t="s">
+        <v>15</v>
+      </c>
+      <c r="N16">
+        <f>MIN(N$3:N$14)</f>
         <v>441</v>
       </c>
     </row>
-    <row r="17" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G17" s="3" t="s">
+    <row r="17" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
         <v>16</v>
       </c>
       <c r="H17">
         <f>MAX(H$3:H$14)</f>
         <v>741</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="J17" t="s">
         <v>16</v>
       </c>
       <c r="K17">
         <f>MAX(K$3:K$14)</f>
+        <v>477</v>
+      </c>
+      <c r="M17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N17">
+        <f>MAX(N$3:N$14)</f>
         <v>502</v>
       </c>
     </row>
-    <row r="18" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G18" s="3" t="s">
+    <row r="18" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="37">
+      <c r="H18" s="33">
         <f>AVERAGE(H$3:H$14)</f>
         <v>550.09090909090912</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="J18" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="37">
+      <c r="K18" s="33">
         <f>AVERAGE(K$3:K$14)</f>
+        <v>455.45454545454544</v>
+      </c>
+      <c r="M18" t="s">
+        <v>17</v>
+      </c>
+      <c r="N18" s="33">
+        <f>AVERAGE(N$3:N$14)</f>
         <v>468.63636363636363</v>
       </c>
     </row>
-    <row r="19" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G19" s="3" t="s">
+    <row r="19" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="37">
+      <c r="H19" s="33">
         <f>STDEV(H$3:H$14)</f>
         <v>83.190690038554905</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="J19" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="37">
+      <c r="K19" s="33">
         <f>STDEV(K$3:K$14)</f>
+        <v>14.801105609809264</v>
+      </c>
+      <c r="M19" t="s">
+        <v>18</v>
+      </c>
+      <c r="N19" s="33">
+        <f>STDEV(N$3:N$14)</f>
         <v>24.146522429835429</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Compared list reps / state by year
</commit_message>
<xml_diff>
--- a/results/Year & Strategy Comparison.xlsx
+++ b/results/Year & Strategy Comparison.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Documents/dev/MM2/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B1B4D6-C128-F745-BD61-AE8510ABA023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801C83AB-0240-CB4A-8E78-D2FBBCCC3D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="500" windowWidth="27680" windowHeight="17500" xr2:uid="{FDB991F3-65B7-2442-88EF-AF8858A1CE50}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Strategies" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>Year</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Strategy 2</t>
+  </si>
+  <si>
+    <t>Strategy 5</t>
   </si>
 </sst>
 </file>
@@ -384,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -423,7 +426,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,13 +742,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5BCF68F-9CA1-1A41-B9FD-C7E5B292FD92}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomRight" activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -757,10 +761,12 @@
     <col min="10" max="11" width="5.83203125" customWidth="1"/>
     <col min="12" max="12" width="5.83203125" style="1" customWidth="1"/>
     <col min="13" max="14" width="5.83203125" customWidth="1"/>
-    <col min="15" max="15" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.83203125" style="1" customWidth="1"/>
+    <col min="16" max="17" width="5.83203125" customWidth="1"/>
+    <col min="18" max="18" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="5"/>
       <c r="C1" s="6" t="s">
@@ -782,10 +788,15 @@
       <c r="M1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="2"/>
-    </row>
-    <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N1" s="6"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="2"/>
+    </row>
+    <row r="2" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -825,14 +836,23 @@
       <c r="M2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="22" t="s">
+      <c r="N2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23">
         <v>2000</v>
       </c>
@@ -872,14 +892,23 @@
       <c r="M3" s="25">
         <v>13</v>
       </c>
-      <c r="N3" s="27">
+      <c r="N3" s="25">
         <v>448</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="26">
+        <v>30</v>
+      </c>
+      <c r="P3" s="25">
+        <v>50</v>
+      </c>
+      <c r="Q3" s="27">
+        <v>485</v>
+      </c>
+      <c r="R3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>2002</v>
       </c>
@@ -907,10 +936,10 @@
       <c r="I4" s="1">
         <v>8</v>
       </c>
-      <c r="J4" s="34">
+      <c r="J4">
         <v>8</v>
       </c>
-      <c r="K4" s="34">
+      <c r="K4">
         <v>443</v>
       </c>
       <c r="L4" s="1">
@@ -919,14 +948,23 @@
       <c r="M4">
         <v>10</v>
       </c>
-      <c r="N4" s="12">
+      <c r="N4" s="35">
         <v>445</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="1">
+        <v>28</v>
+      </c>
+      <c r="P4">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>485</v>
+      </c>
+      <c r="R4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>2004</v>
       </c>
@@ -954,10 +992,10 @@
       <c r="I5" s="1">
         <v>24</v>
       </c>
-      <c r="J5" s="34">
+      <c r="J5">
         <v>24</v>
       </c>
-      <c r="K5" s="34">
+      <c r="K5">
         <v>459</v>
       </c>
       <c r="L5" s="1">
@@ -966,14 +1004,23 @@
       <c r="M5">
         <v>32</v>
       </c>
-      <c r="N5" s="12">
+      <c r="N5" s="35">
         <v>467</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="1">
+        <v>37</v>
+      </c>
+      <c r="P5">
+        <v>50</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>485</v>
+      </c>
+      <c r="R5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>2006</v>
       </c>
@@ -1001,10 +1048,10 @@
       <c r="I6" s="1">
         <v>4</v>
       </c>
-      <c r="J6" s="34">
+      <c r="J6">
         <v>4</v>
       </c>
-      <c r="K6" s="34">
+      <c r="K6">
         <v>439</v>
       </c>
       <c r="L6" s="1">
@@ -1013,14 +1060,23 @@
       <c r="M6">
         <v>6</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N6" s="35">
         <v>441</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="1">
+        <v>29</v>
+      </c>
+      <c r="P6">
+        <v>50</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>485</v>
+      </c>
+      <c r="R6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>2008</v>
       </c>
@@ -1048,10 +1104,10 @@
       <c r="I7" s="1">
         <v>0</v>
       </c>
-      <c r="J7" s="34">
+      <c r="J7">
         <v>29</v>
       </c>
-      <c r="K7" s="34">
+      <c r="K7">
         <v>464</v>
       </c>
       <c r="L7" s="1">
@@ -1060,12 +1116,21 @@
       <c r="M7">
         <v>46</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N7" s="35">
         <v>481</v>
       </c>
-      <c r="O7"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O7" s="1">
+        <v>11</v>
+      </c>
+      <c r="P7">
+        <v>50</v>
+      </c>
+      <c r="Q7" s="12">
+        <v>485</v>
+      </c>
+      <c r="R7"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="28">
         <v>2010</v>
       </c>
@@ -1105,12 +1170,21 @@
       <c r="M8" s="30">
         <v>36</v>
       </c>
-      <c r="N8" s="32">
+      <c r="N8" s="30">
         <v>471</v>
       </c>
-      <c r="O8"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O8" s="31">
+        <v>36</v>
+      </c>
+      <c r="P8" s="30">
+        <v>50</v>
+      </c>
+      <c r="Q8" s="32">
+        <v>485</v>
+      </c>
+      <c r="R8"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>2012</v>
       </c>
@@ -1138,10 +1212,10 @@
       <c r="I9" s="1">
         <v>41</v>
       </c>
-      <c r="J9" s="34">
+      <c r="J9">
         <v>41</v>
       </c>
-      <c r="K9" s="34">
+      <c r="K9">
         <v>476</v>
       </c>
       <c r="L9" s="1">
@@ -1150,12 +1224,21 @@
       <c r="M9">
         <v>67</v>
       </c>
-      <c r="N9" s="12">
+      <c r="N9" s="35">
         <v>502</v>
       </c>
-      <c r="O9"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O9" s="1">
+        <v>45</v>
+      </c>
+      <c r="P9">
+        <v>50</v>
+      </c>
+      <c r="Q9" s="12">
+        <v>485</v>
+      </c>
+      <c r="R9"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>2014</v>
       </c>
@@ -1183,10 +1266,10 @@
       <c r="I10" s="1">
         <v>34</v>
       </c>
-      <c r="J10" s="34">
+      <c r="J10">
         <v>34</v>
       </c>
-      <c r="K10" s="34">
+      <c r="K10">
         <v>469</v>
       </c>
       <c r="L10" s="1">
@@ -1195,12 +1278,21 @@
       <c r="M10">
         <v>67</v>
       </c>
-      <c r="N10" s="12">
+      <c r="N10" s="35">
         <v>502</v>
       </c>
-      <c r="O10"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O10" s="1">
+        <v>42</v>
+      </c>
+      <c r="P10">
+        <v>50</v>
+      </c>
+      <c r="Q10" s="12">
+        <v>485</v>
+      </c>
+      <c r="R10"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>2016</v>
       </c>
@@ -1228,10 +1320,10 @@
       <c r="I11" s="1">
         <v>42</v>
       </c>
-      <c r="J11" s="34">
+      <c r="J11">
         <v>42</v>
       </c>
-      <c r="K11" s="34">
+      <c r="K11">
         <v>477</v>
       </c>
       <c r="L11" s="1">
@@ -1240,12 +1332,21 @@
       <c r="M11">
         <v>64</v>
       </c>
-      <c r="N11" s="12">
+      <c r="N11" s="35">
         <v>499</v>
       </c>
-      <c r="O11"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O11" s="1">
+        <v>46</v>
+      </c>
+      <c r="P11">
+        <v>50</v>
+      </c>
+      <c r="Q11" s="12">
+        <v>485</v>
+      </c>
+      <c r="R11"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>2018</v>
       </c>
@@ -1273,10 +1374,10 @@
       <c r="I12" s="1">
         <v>0</v>
       </c>
-      <c r="J12" s="34">
+      <c r="J12">
         <v>6</v>
       </c>
-      <c r="K12" s="34">
+      <c r="K12">
         <v>441</v>
       </c>
       <c r="L12" s="1">
@@ -1285,14 +1386,23 @@
       <c r="M12">
         <v>19</v>
       </c>
-      <c r="N12" s="12">
+      <c r="N12" s="35">
         <v>454</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O12" s="1">
+        <v>23</v>
+      </c>
+      <c r="P12">
+        <v>50</v>
+      </c>
+      <c r="Q12" s="12">
+        <v>485</v>
+      </c>
+      <c r="R12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="28">
         <v>2020</v>
       </c>
@@ -1332,12 +1442,21 @@
       <c r="M13" s="30">
         <v>10</v>
       </c>
-      <c r="N13" s="32">
+      <c r="N13" s="30">
         <v>445</v>
       </c>
-      <c r="O13"/>
-    </row>
-    <row r="14" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O13" s="31">
+        <v>23</v>
+      </c>
+      <c r="P13" s="30">
+        <v>50</v>
+      </c>
+      <c r="Q13" s="32">
+        <v>485</v>
+      </c>
+      <c r="R13"/>
+    </row>
+    <row r="14" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>2022</v>
       </c>
@@ -1353,10 +1472,13 @@
       <c r="K14" s="15"/>
       <c r="L14" s="16"/>
       <c r="M14" s="15"/>
-      <c r="N14" s="17"/>
-      <c r="O14"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N14" s="15"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="17"/>
+      <c r="R14"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="G16" t="s">
         <v>15</v>
       </c>
@@ -1378,8 +1500,15 @@
         <f>MIN(N$3:N$14)</f>
         <v>441</v>
       </c>
-    </row>
-    <row r="17" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="P16" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q16">
+        <f>MIN(Q$3:Q$14)</f>
+        <v>485</v>
+      </c>
+    </row>
+    <row r="17" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G17" t="s">
         <v>16</v>
       </c>
@@ -1401,8 +1530,15 @@
         <f>MAX(N$3:N$14)</f>
         <v>502</v>
       </c>
-    </row>
-    <row r="18" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="P17" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q17">
+        <f>MAX(Q$3:Q$14)</f>
+        <v>485</v>
+      </c>
+    </row>
+    <row r="18" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G18" t="s">
         <v>17</v>
       </c>
@@ -1417,6 +1553,7 @@
         <f>AVERAGE(K$3:K$14)</f>
         <v>455.45454545454544</v>
       </c>
+      <c r="L18" s="34"/>
       <c r="M18" t="s">
         <v>17</v>
       </c>
@@ -1424,8 +1561,15 @@
         <f>AVERAGE(N$3:N$14)</f>
         <v>468.63636363636363</v>
       </c>
-    </row>
-    <row r="19" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="P18" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q18" s="33">
+        <f>AVERAGE(Q$3:Q$14)</f>
+        <v>485</v>
+      </c>
+    </row>
+    <row r="19" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G19" t="s">
         <v>18</v>
       </c>
@@ -1440,12 +1584,20 @@
         <f>STDEV(K$3:K$14)</f>
         <v>14.801105609809264</v>
       </c>
+      <c r="L19" s="34"/>
       <c r="M19" t="s">
         <v>18</v>
       </c>
       <c r="N19" s="33">
         <f>STDEV(N$3:N$14)</f>
         <v>24.146522429835429</v>
+      </c>
+      <c r="P19" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q19" s="33">
+        <f>STDEV(Q$3:Q$14)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Strategy 5 w/ a fixed list pool size (50) (#3)
* Pulled constants into settings.py

* Added fixed allocation of 50 list seats (5)

* Compared list reps / state by year

* Updated state comparison
</commit_message>
<xml_diff>
--- a/results/Year & Strategy Comparison.xlsx
+++ b/results/Year & Strategy Comparison.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Documents/dev/MM2/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B1B4D6-C128-F745-BD61-AE8510ABA023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801C83AB-0240-CB4A-8E78-D2FBBCCC3D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="500" windowWidth="27680" windowHeight="17500" xr2:uid="{FDB991F3-65B7-2442-88EF-AF8858A1CE50}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Strategies" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>Year</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Strategy 2</t>
+  </si>
+  <si>
+    <t>Strategy 5</t>
   </si>
 </sst>
 </file>
@@ -384,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -423,7 +426,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,13 +742,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5BCF68F-9CA1-1A41-B9FD-C7E5B292FD92}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomRight" activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -757,10 +761,12 @@
     <col min="10" max="11" width="5.83203125" customWidth="1"/>
     <col min="12" max="12" width="5.83203125" style="1" customWidth="1"/>
     <col min="13" max="14" width="5.83203125" customWidth="1"/>
-    <col min="15" max="15" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.83203125" style="1" customWidth="1"/>
+    <col min="16" max="17" width="5.83203125" customWidth="1"/>
+    <col min="18" max="18" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="5"/>
       <c r="C1" s="6" t="s">
@@ -782,10 +788,15 @@
       <c r="M1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="2"/>
-    </row>
-    <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N1" s="6"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="2"/>
+    </row>
+    <row r="2" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -825,14 +836,23 @@
       <c r="M2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="22" t="s">
+      <c r="N2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23">
         <v>2000</v>
       </c>
@@ -872,14 +892,23 @@
       <c r="M3" s="25">
         <v>13</v>
       </c>
-      <c r="N3" s="27">
+      <c r="N3" s="25">
         <v>448</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="26">
+        <v>30</v>
+      </c>
+      <c r="P3" s="25">
+        <v>50</v>
+      </c>
+      <c r="Q3" s="27">
+        <v>485</v>
+      </c>
+      <c r="R3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>2002</v>
       </c>
@@ -907,10 +936,10 @@
       <c r="I4" s="1">
         <v>8</v>
       </c>
-      <c r="J4" s="34">
+      <c r="J4">
         <v>8</v>
       </c>
-      <c r="K4" s="34">
+      <c r="K4">
         <v>443</v>
       </c>
       <c r="L4" s="1">
@@ -919,14 +948,23 @@
       <c r="M4">
         <v>10</v>
       </c>
-      <c r="N4" s="12">
+      <c r="N4" s="35">
         <v>445</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="1">
+        <v>28</v>
+      </c>
+      <c r="P4">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>485</v>
+      </c>
+      <c r="R4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>2004</v>
       </c>
@@ -954,10 +992,10 @@
       <c r="I5" s="1">
         <v>24</v>
       </c>
-      <c r="J5" s="34">
+      <c r="J5">
         <v>24</v>
       </c>
-      <c r="K5" s="34">
+      <c r="K5">
         <v>459</v>
       </c>
       <c r="L5" s="1">
@@ -966,14 +1004,23 @@
       <c r="M5">
         <v>32</v>
       </c>
-      <c r="N5" s="12">
+      <c r="N5" s="35">
         <v>467</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="1">
+        <v>37</v>
+      </c>
+      <c r="P5">
+        <v>50</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>485</v>
+      </c>
+      <c r="R5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>2006</v>
       </c>
@@ -1001,10 +1048,10 @@
       <c r="I6" s="1">
         <v>4</v>
       </c>
-      <c r="J6" s="34">
+      <c r="J6">
         <v>4</v>
       </c>
-      <c r="K6" s="34">
+      <c r="K6">
         <v>439</v>
       </c>
       <c r="L6" s="1">
@@ -1013,14 +1060,23 @@
       <c r="M6">
         <v>6</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N6" s="35">
         <v>441</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="1">
+        <v>29</v>
+      </c>
+      <c r="P6">
+        <v>50</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>485</v>
+      </c>
+      <c r="R6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>2008</v>
       </c>
@@ -1048,10 +1104,10 @@
       <c r="I7" s="1">
         <v>0</v>
       </c>
-      <c r="J7" s="34">
+      <c r="J7">
         <v>29</v>
       </c>
-      <c r="K7" s="34">
+      <c r="K7">
         <v>464</v>
       </c>
       <c r="L7" s="1">
@@ -1060,12 +1116,21 @@
       <c r="M7">
         <v>46</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N7" s="35">
         <v>481</v>
       </c>
-      <c r="O7"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O7" s="1">
+        <v>11</v>
+      </c>
+      <c r="P7">
+        <v>50</v>
+      </c>
+      <c r="Q7" s="12">
+        <v>485</v>
+      </c>
+      <c r="R7"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="28">
         <v>2010</v>
       </c>
@@ -1105,12 +1170,21 @@
       <c r="M8" s="30">
         <v>36</v>
       </c>
-      <c r="N8" s="32">
+      <c r="N8" s="30">
         <v>471</v>
       </c>
-      <c r="O8"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O8" s="31">
+        <v>36</v>
+      </c>
+      <c r="P8" s="30">
+        <v>50</v>
+      </c>
+      <c r="Q8" s="32">
+        <v>485</v>
+      </c>
+      <c r="R8"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>2012</v>
       </c>
@@ -1138,10 +1212,10 @@
       <c r="I9" s="1">
         <v>41</v>
       </c>
-      <c r="J9" s="34">
+      <c r="J9">
         <v>41</v>
       </c>
-      <c r="K9" s="34">
+      <c r="K9">
         <v>476</v>
       </c>
       <c r="L9" s="1">
@@ -1150,12 +1224,21 @@
       <c r="M9">
         <v>67</v>
       </c>
-      <c r="N9" s="12">
+      <c r="N9" s="35">
         <v>502</v>
       </c>
-      <c r="O9"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O9" s="1">
+        <v>45</v>
+      </c>
+      <c r="P9">
+        <v>50</v>
+      </c>
+      <c r="Q9" s="12">
+        <v>485</v>
+      </c>
+      <c r="R9"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>2014</v>
       </c>
@@ -1183,10 +1266,10 @@
       <c r="I10" s="1">
         <v>34</v>
       </c>
-      <c r="J10" s="34">
+      <c r="J10">
         <v>34</v>
       </c>
-      <c r="K10" s="34">
+      <c r="K10">
         <v>469</v>
       </c>
       <c r="L10" s="1">
@@ -1195,12 +1278,21 @@
       <c r="M10">
         <v>67</v>
       </c>
-      <c r="N10" s="12">
+      <c r="N10" s="35">
         <v>502</v>
       </c>
-      <c r="O10"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O10" s="1">
+        <v>42</v>
+      </c>
+      <c r="P10">
+        <v>50</v>
+      </c>
+      <c r="Q10" s="12">
+        <v>485</v>
+      </c>
+      <c r="R10"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>2016</v>
       </c>
@@ -1228,10 +1320,10 @@
       <c r="I11" s="1">
         <v>42</v>
       </c>
-      <c r="J11" s="34">
+      <c r="J11">
         <v>42</v>
       </c>
-      <c r="K11" s="34">
+      <c r="K11">
         <v>477</v>
       </c>
       <c r="L11" s="1">
@@ -1240,12 +1332,21 @@
       <c r="M11">
         <v>64</v>
       </c>
-      <c r="N11" s="12">
+      <c r="N11" s="35">
         <v>499</v>
       </c>
-      <c r="O11"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O11" s="1">
+        <v>46</v>
+      </c>
+      <c r="P11">
+        <v>50</v>
+      </c>
+      <c r="Q11" s="12">
+        <v>485</v>
+      </c>
+      <c r="R11"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>2018</v>
       </c>
@@ -1273,10 +1374,10 @@
       <c r="I12" s="1">
         <v>0</v>
       </c>
-      <c r="J12" s="34">
+      <c r="J12">
         <v>6</v>
       </c>
-      <c r="K12" s="34">
+      <c r="K12">
         <v>441</v>
       </c>
       <c r="L12" s="1">
@@ -1285,14 +1386,23 @@
       <c r="M12">
         <v>19</v>
       </c>
-      <c r="N12" s="12">
+      <c r="N12" s="35">
         <v>454</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O12" s="1">
+        <v>23</v>
+      </c>
+      <c r="P12">
+        <v>50</v>
+      </c>
+      <c r="Q12" s="12">
+        <v>485</v>
+      </c>
+      <c r="R12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="28">
         <v>2020</v>
       </c>
@@ -1332,12 +1442,21 @@
       <c r="M13" s="30">
         <v>10</v>
       </c>
-      <c r="N13" s="32">
+      <c r="N13" s="30">
         <v>445</v>
       </c>
-      <c r="O13"/>
-    </row>
-    <row r="14" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O13" s="31">
+        <v>23</v>
+      </c>
+      <c r="P13" s="30">
+        <v>50</v>
+      </c>
+      <c r="Q13" s="32">
+        <v>485</v>
+      </c>
+      <c r="R13"/>
+    </row>
+    <row r="14" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>2022</v>
       </c>
@@ -1353,10 +1472,13 @@
       <c r="K14" s="15"/>
       <c r="L14" s="16"/>
       <c r="M14" s="15"/>
-      <c r="N14" s="17"/>
-      <c r="O14"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N14" s="15"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="17"/>
+      <c r="R14"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="G16" t="s">
         <v>15</v>
       </c>
@@ -1378,8 +1500,15 @@
         <f>MIN(N$3:N$14)</f>
         <v>441</v>
       </c>
-    </row>
-    <row r="17" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="P16" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q16">
+        <f>MIN(Q$3:Q$14)</f>
+        <v>485</v>
+      </c>
+    </row>
+    <row r="17" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G17" t="s">
         <v>16</v>
       </c>
@@ -1401,8 +1530,15 @@
         <f>MAX(N$3:N$14)</f>
         <v>502</v>
       </c>
-    </row>
-    <row r="18" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="P17" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q17">
+        <f>MAX(Q$3:Q$14)</f>
+        <v>485</v>
+      </c>
+    </row>
+    <row r="18" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G18" t="s">
         <v>17</v>
       </c>
@@ -1417,6 +1553,7 @@
         <f>AVERAGE(K$3:K$14)</f>
         <v>455.45454545454544</v>
       </c>
+      <c r="L18" s="34"/>
       <c r="M18" t="s">
         <v>17</v>
       </c>
@@ -1424,8 +1561,15 @@
         <f>AVERAGE(N$3:N$14)</f>
         <v>468.63636363636363</v>
       </c>
-    </row>
-    <row r="19" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="P18" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q18" s="33">
+        <f>AVERAGE(Q$3:Q$14)</f>
+        <v>485</v>
+      </c>
+    </row>
+    <row r="19" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G19" t="s">
         <v>18</v>
       </c>
@@ -1440,12 +1584,20 @@
         <f>STDEV(K$3:K$14)</f>
         <v>14.801105609809264</v>
       </c>
+      <c r="L19" s="34"/>
       <c r="M19" t="s">
         <v>18</v>
       </c>
       <c r="N19" s="33">
         <f>STDEV(N$3:N$14)</f>
         <v>24.146522429835429</v>
+      </c>
+      <c r="P19" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q19" s="33">
+        <f>STDEV(Q$3:Q$14)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>